<commit_message>
Updated Anonymized Input file
</commit_message>
<xml_diff>
--- a/Input_GTEPJA_Anonymized.xlsx
+++ b/Input_GTEPJA_Anonymized.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Travis\Documents\GitHub\GTEP_SIDS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE45DDC0-8FB7-4B53-9379-B7757310D980}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A0AA281-2AD6-4DD5-8BE1-FF2151C85A73}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="712" firstSheet="18" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" tabRatio="712" firstSheet="11" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Index" sheetId="21" r:id="rId1"/>
@@ -36,9 +36,6 @@
     <sheet name="Par_Scalar" sheetId="12" r:id="rId21"/>
     <sheet name="Par_CalData" sheetId="28" r:id="rId22"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId23"/>
-  </externalReferences>
   <definedNames>
     <definedName name="bll2Btu">Par_Scalar!$C$5</definedName>
     <definedName name="btu">#REF!</definedName>
@@ -465,7 +462,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8452" uniqueCount="624">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8452" uniqueCount="623">
   <si>
     <t>Set_Name</t>
   </si>
@@ -2333,10 +2330,7 @@
     <t>ep31</t>
   </si>
   <si>
-    <t>Set high . Not used in model</t>
-  </si>
-  <si>
-    <t>Set High. Not used in model</t>
+    <t>Set high . Not used in model. Included for future flexibility</t>
   </si>
 </sst>
 </file>
@@ -2838,12 +2832,6 @@
     <xf numFmtId="0" fontId="2" fillId="29" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="30" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="31" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -2854,6 +2842,12 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4480,77 +4474,6 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="Index"/>
-      <sheetName val="Set_Time"/>
-      <sheetName val="Set_Nodes"/>
-      <sheetName val="Set_Plant"/>
-      <sheetName val="Set_TLine"/>
-      <sheetName val="Set_tec"/>
-      <sheetName val="Set_PlantType"/>
-      <sheetName val="Set_MapPlant"/>
-      <sheetName val="Set_Policy"/>
-      <sheetName val="Aliases"/>
-      <sheetName val="Set_MapTline"/>
-      <sheetName val="Par_TLineData"/>
-      <sheetName val="Par_PlantData"/>
-      <sheetName val="Par_AvailabilityFactor"/>
-      <sheetName val="Par_FuelPriceBaseline"/>
-      <sheetName val="Par_FuelPriceLow"/>
-      <sheetName val="Par_FuelPriceHigh"/>
-      <sheetName val="Par_demand"/>
-      <sheetName val="Peak_demand_MW"/>
-      <sheetName val="Par_Scalar"/>
-      <sheetName val="Par_CalData"/>
-      <sheetName val="Par_PolicyRate"/>
-      <sheetName val="Par_Co2Factorkg"/>
-      <sheetName val="par_CO2FactorTon"/>
-      <sheetName val="Par_PTC"/>
-      <sheetName val="par_CTAX"/>
-      <sheetName val="par_InvSubsidy"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
-      <sheetData sheetId="13"/>
-      <sheetData sheetId="14"/>
-      <sheetData sheetId="15"/>
-      <sheetData sheetId="16"/>
-      <sheetData sheetId="17"/>
-      <sheetData sheetId="18"/>
-      <sheetData sheetId="19">
-        <row r="4">
-          <cell r="C4">
-            <v>3.9660000000000002</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="20"/>
-      <sheetData sheetId="21"/>
-      <sheetData sheetId="22"/>
-      <sheetData sheetId="23"/>
-      <sheetData sheetId="24"/>
-      <sheetData sheetId="25"/>
-      <sheetData sheetId="26"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -6292,8 +6215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -7865,7 +7788,7 @@
       <c r="A1" s="26" t="s">
         <v>530</v>
       </c>
-      <c r="B1" s="105"/>
+      <c r="B1" s="103"/>
       <c r="C1" s="27"/>
       <c r="D1" s="27"/>
       <c r="E1" s="27"/>
@@ -7891,28 +7814,28 @@
       <c r="Y1" s="27"/>
       <c r="Z1" s="27"/>
       <c r="AA1" s="27"/>
-      <c r="AB1" s="105"/>
+      <c r="AB1" s="103"/>
     </row>
     <row r="2" spans="1:28" ht="86.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="106" t="s">
+      <c r="B2" s="104" t="s">
         <v>331</v>
       </c>
-      <c r="C2" s="107" t="s">
+      <c r="C2" s="105" t="s">
         <v>140</v>
       </c>
-      <c r="D2" s="107" t="s">
+      <c r="D2" s="105" t="s">
         <v>143</v>
       </c>
-      <c r="E2" s="107" t="s">
+      <c r="E2" s="105" t="s">
         <v>141</v>
       </c>
-      <c r="F2" s="107" t="s">
+      <c r="F2" s="105" t="s">
         <v>146</v>
       </c>
-      <c r="G2" s="107" t="s">
+      <c r="G2" s="105" t="s">
         <v>319</v>
       </c>
       <c r="H2" s="36" t="s">
@@ -7921,7 +7844,7 @@
       <c r="I2" s="36" t="s">
         <v>139</v>
       </c>
-      <c r="J2" s="107" t="s">
+      <c r="J2" s="105" t="s">
         <v>131</v>
       </c>
       <c r="K2" s="36" t="s">
@@ -7948,22 +7871,22 @@
       <c r="R2" s="36" t="s">
         <v>184</v>
       </c>
-      <c r="S2" s="108" t="s">
+      <c r="S2" s="106" t="s">
         <v>185</v>
       </c>
-      <c r="T2" s="108" t="s">
+      <c r="T2" s="106" t="s">
         <v>186</v>
       </c>
-      <c r="U2" s="107" t="s">
+      <c r="U2" s="105" t="s">
         <v>183</v>
       </c>
-      <c r="V2" s="107" t="s">
+      <c r="V2" s="105" t="s">
         <v>132</v>
       </c>
-      <c r="W2" s="107" t="s">
+      <c r="W2" s="105" t="s">
         <v>309</v>
       </c>
-      <c r="X2" s="108" t="s">
+      <c r="X2" s="106" t="s">
         <v>133</v>
       </c>
       <c r="Y2" s="36" t="s">
@@ -7972,10 +7895,10 @@
       <c r="Z2" s="36" t="s">
         <v>161</v>
       </c>
-      <c r="AA2" s="107" t="s">
+      <c r="AA2" s="105" t="s">
         <v>172</v>
       </c>
-      <c r="AB2" s="106" t="s">
+      <c r="AB2" s="104" t="s">
         <v>1</v>
       </c>
     </row>
@@ -8006,28 +7929,28 @@
       <c r="J3" s="28" t="s">
         <v>134</v>
       </c>
-      <c r="K3" s="104" t="s">
+      <c r="K3" s="102" t="s">
         <v>156</v>
       </c>
-      <c r="L3" s="104" t="s">
+      <c r="L3" s="102" t="s">
         <v>157</v>
       </c>
-      <c r="M3" s="104" t="s">
+      <c r="M3" s="102" t="s">
         <v>323</v>
       </c>
-      <c r="N3" s="104" t="s">
+      <c r="N3" s="102" t="s">
         <v>324</v>
       </c>
-      <c r="O3" s="104" t="s">
+      <c r="O3" s="102" t="s">
         <v>325</v>
       </c>
       <c r="P3" s="36" t="s">
         <v>275</v>
       </c>
-      <c r="Q3" s="104" t="s">
+      <c r="Q3" s="102" t="s">
         <v>326</v>
       </c>
-      <c r="R3" s="104" t="s">
+      <c r="R3" s="102" t="s">
         <v>327</v>
       </c>
       <c r="S3" s="28" t="s">
@@ -8065,7 +7988,7 @@
       <c r="A4" s="8" t="s">
         <v>591</v>
       </c>
-      <c r="B4" s="104" t="s">
+      <c r="B4" s="102" t="s">
         <v>155</v>
       </c>
       <c r="C4" s="27">
@@ -8109,7 +8032,7 @@
         <v>2585.7016530197538</v>
       </c>
       <c r="P4" s="27">
-        <f>O4*[1]Par_Scalar!$C$4</f>
+        <f>O4*Par_Scalar!$C$4</f>
         <v>10254.892755876344</v>
       </c>
       <c r="Q4" s="29">
@@ -8144,7 +8067,7 @@
         <v>2020</v>
       </c>
       <c r="AA4" s="27"/>
-      <c r="AB4" s="104" t="s">
+      <c r="AB4" s="102" t="s">
         <v>154</v>
       </c>
     </row>
@@ -8152,7 +8075,7 @@
       <c r="A5" s="8" t="s">
         <v>592</v>
       </c>
-      <c r="B5" s="104" t="s">
+      <c r="B5" s="102" t="s">
         <v>155</v>
       </c>
       <c r="C5" s="27">
@@ -8196,7 +8119,7 @@
         <v>2762.578562559012</v>
       </c>
       <c r="P5" s="27">
-        <f>O5*[1]Par_Scalar!$C$4</f>
+        <f>O5*Par_Scalar!$C$4</f>
         <v>10956.386579109041</v>
       </c>
       <c r="Q5" s="29">
@@ -8231,7 +8154,7 @@
         <v>2020</v>
       </c>
       <c r="AA5" s="27"/>
-      <c r="AB5" s="104" t="s">
+      <c r="AB5" s="102" t="s">
         <v>154</v>
       </c>
     </row>
@@ -8239,7 +8162,7 @@
       <c r="A6" s="8" t="s">
         <v>593</v>
       </c>
-      <c r="B6" s="104" t="s">
+      <c r="B6" s="102" t="s">
         <v>155</v>
       </c>
       <c r="C6" s="27">
@@ -8283,7 +8206,7 @@
         <v>2677.7388430327214</v>
       </c>
       <c r="P6" s="27">
-        <f>O6*[1]Par_Scalar!$C$4</f>
+        <f>O6*Par_Scalar!$C$4</f>
         <v>10619.912251467773</v>
       </c>
       <c r="Q6" s="29">
@@ -8318,7 +8241,7 @@
         <v>2020</v>
       </c>
       <c r="AA6" s="27"/>
-      <c r="AB6" s="104" t="s">
+      <c r="AB6" s="102" t="s">
         <v>154</v>
       </c>
     </row>
@@ -8326,7 +8249,7 @@
       <c r="A7" s="8" t="s">
         <v>594</v>
       </c>
-      <c r="B7" s="104" t="s">
+      <c r="B7" s="102" t="s">
         <v>155</v>
       </c>
       <c r="C7" s="27">
@@ -8370,7 +8293,7 @@
         <v>2828.7403088055112</v>
       </c>
       <c r="P7" s="27">
-        <f>O7*[1]Par_Scalar!$C$4</f>
+        <f>O7*Par_Scalar!$C$4</f>
         <v>11218.784064722659</v>
       </c>
       <c r="Q7" s="27">
@@ -8405,7 +8328,7 @@
         <v>2020</v>
       </c>
       <c r="AA7" s="27"/>
-      <c r="AB7" s="104" t="s">
+      <c r="AB7" s="102" t="s">
         <v>154</v>
       </c>
     </row>
@@ -8413,7 +8336,7 @@
       <c r="A8" s="8" t="s">
         <v>595</v>
       </c>
-      <c r="B8" s="104" t="s">
+      <c r="B8" s="102" t="s">
         <v>155</v>
       </c>
       <c r="C8" s="27">
@@ -8457,7 +8380,7 @@
         <v>1962.3239403791908</v>
       </c>
       <c r="P8" s="27">
-        <f>O8*[1]Par_Scalar!$C$4</f>
+        <f>O8*Par_Scalar!$C$4</f>
         <v>7782.5767475438715</v>
       </c>
       <c r="Q8" s="27">
@@ -8490,7 +8413,7 @@
       </c>
       <c r="Z8" s="27"/>
       <c r="AA8" s="27"/>
-      <c r="AB8" s="104" t="s">
+      <c r="AB8" s="102" t="s">
         <v>163</v>
       </c>
     </row>
@@ -8498,7 +8421,7 @@
       <c r="A9" s="8" t="s">
         <v>596</v>
       </c>
-      <c r="B9" s="104" t="s">
+      <c r="B9" s="102" t="s">
         <v>155</v>
       </c>
       <c r="C9" s="27">
@@ -8542,7 +8465,7 @@
         <v>1965.3066225211198</v>
       </c>
       <c r="P9" s="27">
-        <f>O9*[1]Par_Scalar!$C$4</f>
+        <f>O9*Par_Scalar!$C$4</f>
         <v>7794.4060649187613</v>
       </c>
       <c r="Q9" s="27">
@@ -8575,7 +8498,7 @@
       </c>
       <c r="Z9" s="27"/>
       <c r="AA9" s="27"/>
-      <c r="AB9" s="104" t="s">
+      <c r="AB9" s="102" t="s">
         <v>163</v>
       </c>
     </row>
@@ -8583,7 +8506,7 @@
       <c r="A10" s="8" t="s">
         <v>597</v>
       </c>
-      <c r="B10" s="104" t="s">
+      <c r="B10" s="102" t="s">
         <v>165</v>
       </c>
       <c r="C10" s="27">
@@ -8627,7 +8550,7 @@
         <v>2348.2426813974903</v>
       </c>
       <c r="P10" s="27">
-        <f>O10*[1]Par_Scalar!$C$4</f>
+        <f>O10*Par_Scalar!$C$4</f>
         <v>9313.1304744224472</v>
       </c>
       <c r="Q10" s="27">
@@ -8660,7 +8583,7 @@
       </c>
       <c r="Z10" s="27"/>
       <c r="AA10" s="27"/>
-      <c r="AB10" s="104" t="s">
+      <c r="AB10" s="102" t="s">
         <v>164</v>
       </c>
     </row>
@@ -8668,7 +8591,7 @@
       <c r="A11" s="8" t="s">
         <v>598</v>
       </c>
-      <c r="B11" s="104" t="s">
+      <c r="B11" s="102" t="s">
         <v>165</v>
       </c>
       <c r="C11" s="27">
@@ -8712,7 +8635,7 @@
         <v>2423.8234637339324</v>
       </c>
       <c r="P11" s="27">
-        <f>O11*[1]Par_Scalar!$C$4</f>
+        <f>O11*Par_Scalar!$C$4</f>
         <v>9612.8838571687756</v>
       </c>
       <c r="Q11" s="27">
@@ -8745,7 +8668,7 @@
       </c>
       <c r="Z11" s="27"/>
       <c r="AA11" s="27"/>
-      <c r="AB11" s="104" t="s">
+      <c r="AB11" s="102" t="s">
         <v>164</v>
       </c>
     </row>
@@ -8753,7 +8676,7 @@
       <c r="A12" s="8" t="s">
         <v>599</v>
       </c>
-      <c r="B12" s="104" t="s">
+      <c r="B12" s="102" t="s">
         <v>165</v>
       </c>
       <c r="C12" s="27">
@@ -8797,7 +8720,7 @@
         <v>2769.2321909956445</v>
       </c>
       <c r="P12" s="27">
-        <f>O12*[1]Par_Scalar!$C$4</f>
+        <f>O12*Par_Scalar!$C$4</f>
         <v>10982.774869488727</v>
       </c>
       <c r="Q12" s="27">
@@ -8830,7 +8753,7 @@
       </c>
       <c r="Z12" s="27"/>
       <c r="AA12" s="27"/>
-      <c r="AB12" s="104" t="s">
+      <c r="AB12" s="102" t="s">
         <v>164</v>
       </c>
     </row>
@@ -8838,7 +8761,7 @@
       <c r="A13" s="8" t="s">
         <v>600</v>
       </c>
-      <c r="B13" s="104" t="s">
+      <c r="B13" s="102" t="s">
         <v>165</v>
       </c>
       <c r="C13" s="27">
@@ -8882,7 +8805,7 @@
         <v>3250.8925455664371</v>
       </c>
       <c r="P13" s="27">
-        <f>O13*[1]Par_Scalar!$C$4</f>
+        <f>O13*Par_Scalar!$C$4</f>
         <v>12893.03983571649</v>
       </c>
       <c r="Q13" s="27">
@@ -8915,7 +8838,7 @@
       </c>
       <c r="Z13" s="27"/>
       <c r="AA13" s="27"/>
-      <c r="AB13" s="104" t="s">
+      <c r="AB13" s="102" t="s">
         <v>164</v>
       </c>
     </row>
@@ -8923,7 +8846,7 @@
       <c r="A14" s="8" t="s">
         <v>601</v>
       </c>
-      <c r="B14" s="104" t="s">
+      <c r="B14" s="102" t="s">
         <v>165</v>
       </c>
       <c r="C14" s="27">
@@ -8967,7 +8890,7 @@
         <v>3325.269506039765</v>
       </c>
       <c r="P14" s="27">
-        <f>O14*[1]Par_Scalar!$C$4</f>
+        <f>O14*Par_Scalar!$C$4</f>
         <v>13188.018860953709</v>
       </c>
       <c r="Q14" s="27">
@@ -9000,7 +8923,7 @@
       </c>
       <c r="Z14" s="27"/>
       <c r="AA14" s="27"/>
-      <c r="AB14" s="104" t="s">
+      <c r="AB14" s="102" t="s">
         <v>164</v>
       </c>
     </row>
@@ -9008,7 +8931,7 @@
       <c r="A15" s="8" t="s">
         <v>602</v>
       </c>
-      <c r="B15" s="104" t="s">
+      <c r="B15" s="102" t="s">
         <v>165</v>
       </c>
       <c r="C15" s="27">
@@ -9052,7 +8975,7 @@
         <v>2975.4606487237302</v>
       </c>
       <c r="P15" s="27">
-        <f>O15*[1]Par_Scalar!$C$4</f>
+        <f>O15*Par_Scalar!$C$4</f>
         <v>11800.676932838314</v>
       </c>
       <c r="Q15" s="27">
@@ -9085,7 +9008,7 @@
       </c>
       <c r="Z15" s="27"/>
       <c r="AA15" s="27"/>
-      <c r="AB15" s="104" t="s">
+      <c r="AB15" s="102" t="s">
         <v>164</v>
       </c>
     </row>
@@ -9137,7 +9060,7 @@
         <v>2218.5084690979452</v>
       </c>
       <c r="P16" s="75">
-        <f>O16*[1]Par_Scalar!$C$4</f>
+        <f>O16*Par_Scalar!$C$4</f>
         <v>8798.6045884424511</v>
       </c>
       <c r="Q16" s="75">
@@ -9180,7 +9103,7 @@
       <c r="A17" s="8" t="s">
         <v>604</v>
       </c>
-      <c r="B17" s="104" t="s">
+      <c r="B17" s="102" t="s">
         <v>175</v>
       </c>
       <c r="C17" s="27">
@@ -9224,7 +9147,7 @@
         <v>1858.1805857726356</v>
       </c>
       <c r="P17" s="27">
-        <f>O17*[1]Par_Scalar!$C$4</f>
+        <f>O17*Par_Scalar!$C$4</f>
         <v>7369.5442031742732</v>
       </c>
       <c r="Q17" s="27">
@@ -9257,7 +9180,7 @@
       </c>
       <c r="Z17" s="27"/>
       <c r="AA17" s="27"/>
-      <c r="AB17" s="104" t="s">
+      <c r="AB17" s="102" t="s">
         <v>166</v>
       </c>
     </row>
@@ -9265,7 +9188,7 @@
       <c r="A18" s="8" t="s">
         <v>605</v>
       </c>
-      <c r="B18" s="104" t="s">
+      <c r="B18" s="102" t="s">
         <v>155</v>
       </c>
       <c r="C18" s="27">
@@ -9309,7 +9232,7 @@
         <v>1891.7304015296365</v>
       </c>
       <c r="P18" s="27">
-        <f>O18*[1]Par_Scalar!$C$4</f>
+        <f>O18*Par_Scalar!$C$4</f>
         <v>7502.6027724665391</v>
       </c>
       <c r="Q18" s="27">
@@ -9343,7 +9266,7 @@
         <v>2024</v>
       </c>
       <c r="AA18" s="27"/>
-      <c r="AB18" s="104" t="s">
+      <c r="AB18" s="102" t="s">
         <v>163</v>
       </c>
     </row>
@@ -9351,7 +9274,7 @@
       <c r="A19" s="8" t="s">
         <v>606</v>
       </c>
-      <c r="B19" s="104" t="s">
+      <c r="B19" s="102" t="s">
         <v>155</v>
       </c>
       <c r="C19" s="27">
@@ -9395,7 +9318,7 @@
         <v>2059.034416826004</v>
       </c>
       <c r="P19" s="27">
-        <f>O19*[1]Par_Scalar!$C$4</f>
+        <f>O19*Par_Scalar!$C$4</f>
         <v>8166.1304971319323</v>
       </c>
       <c r="Q19" s="27">
@@ -9430,7 +9353,7 @@
         <v>2026</v>
       </c>
       <c r="AA19" s="27"/>
-      <c r="AB19" s="104" t="s">
+      <c r="AB19" s="102" t="s">
         <v>167</v>
       </c>
     </row>
@@ -9438,7 +9361,7 @@
       <c r="A20" s="8" t="s">
         <v>607</v>
       </c>
-      <c r="B20" s="104" t="s">
+      <c r="B20" s="102" t="s">
         <v>155</v>
       </c>
       <c r="C20" s="27">
@@ -9482,7 +9405,7 @@
         <v>2048.0401529636711</v>
       </c>
       <c r="P20" s="27">
-        <f>O20*[1]Par_Scalar!$C$4</f>
+        <f>O20*Par_Scalar!$C$4</f>
         <v>8122.52724665392</v>
       </c>
       <c r="Q20" s="27">
@@ -9517,7 +9440,7 @@
         <v>2032</v>
       </c>
       <c r="AA20" s="27"/>
-      <c r="AB20" s="104" t="s">
+      <c r="AB20" s="102" t="s">
         <v>167</v>
       </c>
     </row>
@@ -9525,7 +9448,7 @@
       <c r="A21" s="8" t="s">
         <v>608</v>
       </c>
-      <c r="B21" s="104" t="s">
+      <c r="B21" s="102" t="s">
         <v>155</v>
       </c>
       <c r="C21" s="27">
@@ -9567,7 +9490,7 @@
         <v>2270.5544933078395</v>
       </c>
       <c r="P21" s="27">
-        <f>O21*[1]Par_Scalar!$C$4</f>
+        <f>O21*Par_Scalar!$C$4</f>
         <v>9005.0191204588918</v>
       </c>
       <c r="Q21" s="27">
@@ -9600,7 +9523,7 @@
       </c>
       <c r="Z21" s="27"/>
       <c r="AA21" s="27"/>
-      <c r="AB21" s="104" t="s">
+      <c r="AB21" s="102" t="s">
         <v>168</v>
       </c>
     </row>
@@ -10050,7 +9973,7 @@
       <c r="AA27" s="27">
         <v>2.5</v>
       </c>
-      <c r="AB27" s="104" t="s">
+      <c r="AB27" s="102" t="s">
         <v>169</v>
       </c>
     </row>
@@ -14257,7 +14180,7 @@
       <c r="A2" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="106" t="s">
+      <c r="B2" s="104" t="s">
         <v>331</v>
       </c>
     </row>
@@ -15636,12 +15559,12 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="102" t="s">
+      <c r="A2" s="107" t="s">
         <v>535</v>
       </c>
-      <c r="B2" s="102"/>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
+      <c r="B2" s="107"/>
+      <c r="C2" s="107"/>
+      <c r="D2" s="107"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
@@ -16178,12 +16101,12 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="108" t="s">
         <v>536</v>
       </c>
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
@@ -16719,12 +16642,12 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="103" t="s">
+      <c r="A2" s="108" t="s">
         <v>537</v>
       </c>
-      <c r="B2" s="103"/>
-      <c r="C2" s="103"/>
-      <c r="D2" s="103"/>
+      <c r="B2" s="108"/>
+      <c r="C2" s="108"/>
+      <c r="D2" s="108"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
@@ -76846,7 +76769,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -76955,7 +76878,7 @@
         <v>999999999999</v>
       </c>
       <c r="D9" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.55000000000000004">
@@ -77002,8 +76925,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -78577,7 +78500,7 @@
       <c r="A3" s="8" t="s">
         <v>591</v>
       </c>
-      <c r="B3" s="104" t="s">
+      <c r="B3" s="102" t="s">
         <v>155</v>
       </c>
     </row>
@@ -78585,7 +78508,7 @@
       <c r="A4" s="8" t="s">
         <v>592</v>
       </c>
-      <c r="B4" s="104" t="s">
+      <c r="B4" s="102" t="s">
         <v>155</v>
       </c>
     </row>
@@ -78593,7 +78516,7 @@
       <c r="A5" s="8" t="s">
         <v>593</v>
       </c>
-      <c r="B5" s="104" t="s">
+      <c r="B5" s="102" t="s">
         <v>155</v>
       </c>
     </row>
@@ -78601,7 +78524,7 @@
       <c r="A6" s="8" t="s">
         <v>594</v>
       </c>
-      <c r="B6" s="104" t="s">
+      <c r="B6" s="102" t="s">
         <v>155</v>
       </c>
     </row>
@@ -78609,7 +78532,7 @@
       <c r="A7" s="8" t="s">
         <v>595</v>
       </c>
-      <c r="B7" s="104" t="s">
+      <c r="B7" s="102" t="s">
         <v>155</v>
       </c>
     </row>
@@ -78617,7 +78540,7 @@
       <c r="A8" s="8" t="s">
         <v>596</v>
       </c>
-      <c r="B8" s="104" t="s">
+      <c r="B8" s="102" t="s">
         <v>155</v>
       </c>
     </row>
@@ -78625,7 +78548,7 @@
       <c r="A9" s="8" t="s">
         <v>597</v>
       </c>
-      <c r="B9" s="104" t="s">
+      <c r="B9" s="102" t="s">
         <v>165</v>
       </c>
     </row>
@@ -78633,7 +78556,7 @@
       <c r="A10" s="8" t="s">
         <v>598</v>
       </c>
-      <c r="B10" s="104" t="s">
+      <c r="B10" s="102" t="s">
         <v>165</v>
       </c>
     </row>
@@ -78641,7 +78564,7 @@
       <c r="A11" s="8" t="s">
         <v>599</v>
       </c>
-      <c r="B11" s="104" t="s">
+      <c r="B11" s="102" t="s">
         <v>165</v>
       </c>
     </row>
@@ -78649,7 +78572,7 @@
       <c r="A12" s="8" t="s">
         <v>600</v>
       </c>
-      <c r="B12" s="104" t="s">
+      <c r="B12" s="102" t="s">
         <v>165</v>
       </c>
     </row>
@@ -78657,7 +78580,7 @@
       <c r="A13" s="8" t="s">
         <v>601</v>
       </c>
-      <c r="B13" s="104" t="s">
+      <c r="B13" s="102" t="s">
         <v>165</v>
       </c>
     </row>
@@ -78665,7 +78588,7 @@
       <c r="A14" s="8" t="s">
         <v>602</v>
       </c>
-      <c r="B14" s="104" t="s">
+      <c r="B14" s="102" t="s">
         <v>165</v>
       </c>
     </row>
@@ -78681,7 +78604,7 @@
       <c r="A16" s="8" t="s">
         <v>604</v>
       </c>
-      <c r="B16" s="104" t="s">
+      <c r="B16" s="102" t="s">
         <v>175</v>
       </c>
     </row>
@@ -78689,7 +78612,7 @@
       <c r="A17" s="8" t="s">
         <v>605</v>
       </c>
-      <c r="B17" s="104" t="s">
+      <c r="B17" s="102" t="s">
         <v>155</v>
       </c>
     </row>
@@ -78697,7 +78620,7 @@
       <c r="A18" s="8" t="s">
         <v>606</v>
       </c>
-      <c r="B18" s="104" t="s">
+      <c r="B18" s="102" t="s">
         <v>155</v>
       </c>
     </row>
@@ -78705,7 +78628,7 @@
       <c r="A19" s="8" t="s">
         <v>607</v>
       </c>
-      <c r="B19" s="104" t="s">
+      <c r="B19" s="102" t="s">
         <v>155</v>
       </c>
     </row>
@@ -78713,7 +78636,7 @@
       <c r="A20" s="8" t="s">
         <v>608</v>
       </c>
-      <c r="B20" s="104" t="s">
+      <c r="B20" s="102" t="s">
         <v>155</v>
       </c>
     </row>

</xml_diff>